<commit_message>
Reviewed test notes and profile. Updated names, made test more descriptive and clear.
</commit_message>
<xml_diff>
--- a/profile.xlsx
+++ b/profile.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9E0B3540-8ED0-4ADE-975D-8ED20D8C5DFC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCB0928-AE78-0146-BB78-47CB63A19CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15600" yWindow="-24000" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Required Tasks" sheetId="2" r:id="rId1"/>
     <sheet name="Desirable Tasks" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -50,9 +58,6 @@
     <t>Reels</t>
   </si>
   <si>
-    <t>WinRules</t>
-  </si>
-  <si>
     <t>3 x ACE</t>
   </si>
   <si>
@@ -65,9 +70,6 @@
     <t>3 x JACK</t>
   </si>
   <si>
-    <t>rule</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -81,17 +83,24 @@
   </si>
   <si>
     <t>99% confidence level</t>
+  </si>
+  <si>
+    <t>Rule/ Pattern</t>
+  </si>
+  <si>
+    <t>Win patterns</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000000%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.000000000000000"/>
     <numFmt numFmtId="167" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="168" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -299,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -384,16 +393,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -421,6 +424,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -705,27 +723,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD3AD2D-3434-41F3-84D8-191D3A618518}">
   <dimension ref="B1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="39" t="s">
+    <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="40"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -733,11 +751,11 @@
         <v>6</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="43">
         <v>0</v>
       </c>
       <c r="C4" s="6">
@@ -746,11 +764,11 @@
       <c r="D4" s="24">
         <v>3.9969188132860543E-3</v>
       </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+      <c r="I4" s="33"/>
+      <c r="J4" s="34"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="43">
         <v>1</v>
       </c>
       <c r="C5" s="6">
@@ -759,11 +777,11 @@
       <c r="D5" s="24">
         <v>3.7387752005168754E-3</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="36"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="43">
         <v>2</v>
       </c>
       <c r="C6" s="6">
@@ -772,11 +790,11 @@
       <c r="D6" s="24">
         <v>3.2634705452937677E-3</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="36"/>
-    </row>
-    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="4">
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
+    </row>
+    <row r="7" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44">
         <v>3</v>
       </c>
       <c r="C7" s="7">
@@ -785,31 +803,31 @@
       <c r="D7" s="25">
         <v>2.4476029089703253E-3</v>
       </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="36"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I10" s="35"/>
-      <c r="J10" s="36"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I11" s="35"/>
-      <c r="J11" s="36"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I13" s="35"/>
-      <c r="J13" s="36"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I14" s="35"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="34"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I10" s="33"/>
+      <c r="J10" s="34"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I11" s="33"/>
+      <c r="J11" s="34"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I12" s="33"/>
+      <c r="J12" s="34"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I13" s="33"/>
+      <c r="J13" s="34"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I14" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -824,39 +842,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA5516A-90F7-4B36-B07D-D0DE0F7285C7}">
   <dimension ref="B1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43"/>
-      <c r="I2" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="44"/>
-      <c r="K2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="I2" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="42"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
@@ -872,19 +890,19 @@
         <v>2</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
@@ -902,19 +920,19 @@
         <v>3</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="30">
+        <v>9</v>
+      </c>
+      <c r="J4" s="45">
         <v>15</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="30">
         <v>4.6296296296296294E-3</v>
       </c>
-      <c r="L4" s="34">
+      <c r="L4" s="32">
         <v>5.5384110459210452E-4</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
@@ -932,9 +950,9 @@
         <v>3</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="11">
+        <v>10</v>
+      </c>
+      <c r="J5" s="46">
         <v>14</v>
       </c>
       <c r="K5" s="24">
@@ -944,7 +962,7 @@
         <v>8.499723604911371E-4</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>3</v>
       </c>
@@ -962,9 +980,9 @@
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="11">
+        <v>11</v>
+      </c>
+      <c r="J6" s="46">
         <v>13</v>
       </c>
       <c r="K6" s="24">
@@ -974,7 +992,7 @@
         <v>1.1815745644745545E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D7" s="23">
         <v>3</v>
       </c>
@@ -988,9 +1006,9 @@
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="11">
+        <v>12</v>
+      </c>
+      <c r="J7" s="46">
         <v>12</v>
       </c>
       <c r="K7" s="24">
@@ -1000,7 +1018,7 @@
         <v>1.5407870363415006E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D8" s="23">
         <v>4</v>
       </c>
@@ -1013,10 +1031,10 @@
       <c r="G8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="33">
+      <c r="I8" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="47">
         <v>11</v>
       </c>
       <c r="K8" s="25">
@@ -1026,7 +1044,7 @@
         <v>2.0740041117499153E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D9" s="23">
         <v>5</v>
       </c>
@@ -1040,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D10" s="23">
         <v>6</v>
       </c>
@@ -1054,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D11" s="23">
         <v>7</v>
       </c>
@@ -1068,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D12" s="23">
         <v>8</v>
       </c>
@@ -1082,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D13" s="23">
         <v>9</v>
       </c>
@@ -1096,7 +1114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D14" s="23">
         <v>10</v>
       </c>
@@ -1110,7 +1128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D15" s="23">
         <v>11</v>
       </c>
@@ -1124,7 +1142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D16" s="23">
         <v>12</v>
       </c>
@@ -1138,7 +1156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D17" s="23">
         <v>13</v>
       </c>
@@ -1152,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D18" s="23">
         <v>14</v>
       </c>
@@ -1166,7 +1184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D19" s="23">
         <v>15</v>
       </c>
@@ -1180,7 +1198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D20" s="23">
         <v>16</v>
       </c>
@@ -1194,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="15">
         <v>17</v>
       </c>
@@ -1208,13 +1226,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:16" x14ac:dyDescent="0.2">
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:16" x14ac:dyDescent="0.2">
       <c r="P31" s="1"/>
     </row>
-    <row r="41" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O41" s="22"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made sure it opens on first tab
</commit_message>
<xml_diff>
--- a/profile.xlsx
+++ b/profile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCB0928-AE78-0146-BB78-47CB63A19CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64F0633-1B38-1442-8DE1-67363341613F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="-24000" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15600" yWindow="-23540" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Required Tasks" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
   <si>
     <t>ACE</t>
   </si>
@@ -70,12 +70,6 @@
     <t>3 x JACK</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>expected chance</t>
-  </si>
-  <si>
     <t>2 x ACE</t>
   </si>
   <si>
@@ -89,6 +83,9 @@
   </si>
   <si>
     <t>Win patterns</t>
+  </si>
+  <si>
+    <t>Expected chance</t>
   </si>
 </sst>
 </file>
@@ -408,6 +405,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,21 +436,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -723,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD3AD2D-3434-41F3-84D8-191D3A618518}">
   <dimension ref="B1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -735,12 +732,12 @@
   <sheetData>
     <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -751,11 +748,11 @@
         <v>6</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="43">
+      <c r="B4" s="37">
         <v>0</v>
       </c>
       <c r="C4" s="6">
@@ -768,7 +765,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="43">
+      <c r="B5" s="37">
         <v>1</v>
       </c>
       <c r="C5" s="6">
@@ -781,7 +778,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="43">
+      <c r="B6" s="37">
         <v>2</v>
       </c>
       <c r="C6" s="6">
@@ -794,7 +791,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44">
+      <c r="B7" s="38">
         <v>3</v>
       </c>
       <c r="C7" s="7">
@@ -842,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA5516A-90F7-4B36-B07D-D0DE0F7285C7}">
   <dimension ref="B1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -860,18 +857,18 @@
         <v>7</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
-      <c r="I2" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="38"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="I2" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="47"/>
+      <c r="K2" s="43"/>
       <c r="L2" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -890,16 +887,16 @@
         <v>2</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="14" t="s">
         <v>14</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
@@ -922,7 +919,7 @@
       <c r="I4" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="45">
+      <c r="J4" s="39">
         <v>15</v>
       </c>
       <c r="K4" s="30">
@@ -952,7 +949,7 @@
       <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="46">
+      <c r="J5" s="40">
         <v>14</v>
       </c>
       <c r="K5" s="24">
@@ -982,7 +979,7 @@
       <c r="I6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="46">
+      <c r="J6" s="40">
         <v>13</v>
       </c>
       <c r="K6" s="24">
@@ -1008,7 +1005,7 @@
       <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="46">
+      <c r="J7" s="40">
         <v>12</v>
       </c>
       <c r="K7" s="24">
@@ -1032,9 +1029,9 @@
         <v>0</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="47">
+        <v>13</v>
+      </c>
+      <c r="J8" s="41">
         <v>11</v>
       </c>
       <c r="K8" s="25">

</xml_diff>